<commit_message>
feat: handle On Hit and Die event
</commit_message>
<xml_diff>
--- a/Excels/GameData.xlsx
+++ b/Excels/GameData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCMUS\Nam 4\Game\2D\The Transcendent Legend 2D\The Transcendent Legend 2D\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A597FBD4-FCA0-491F-9AA3-D38EEB780AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAF276A-7FAE-4C64-88EF-45D1B390322B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,8 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -46,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
   <si>
     <t>Id</t>
   </si>
@@ -175,6 +173,9 @@
   </si>
   <si>
     <t>SelfDamage</t>
+  </si>
+  <si>
+    <t>Health</t>
   </si>
 </sst>
 </file>
@@ -353,10 +354,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -370,6 +370,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1046,10 +1049,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1060,321 +1063,312 @@
     <col min="9" max="9" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="M1" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="12">
         <v>1</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="12">
         <v>1</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="12">
         <v>0</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="12">
         <v>1</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="12">
         <v>1</v>
       </c>
-      <c r="I2" s="13">
+      <c r="I2" s="12">
         <v>2</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="12">
         <v>80</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="12">
         <v>150</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
-        <v>2</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="15"/>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
-        <v>3</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="15"/>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
-        <v>4</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="15"/>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
-        <v>5</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="15"/>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
-        <v>6</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="15"/>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
-        <v>7</v>
-      </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="15"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
-        <v>8</v>
-      </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="15"/>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
-        <v>9</v>
-      </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="15"/>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
-        <v>10</v>
-      </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="15"/>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
-        <v>11</v>
-      </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="15"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="15"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
-        <v>13</v>
-      </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="15"/>
-    </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
-        <v>14</v>
-      </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="15"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13">
-        <v>15</v>
-      </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="15"/>
-    </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
-        <v>16</v>
-      </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="15"/>
+      <c r="M2" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1443,266 +1437,266 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2">
         <v>10</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1764,248 +1758,248 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2">
         <v>10</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2054,182 +2048,182 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2">
         <v>10</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2258,296 +2252,296 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>10</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>0</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>1</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>0</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="4">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>10</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>0</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>5</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>2</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="4">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="5"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="5"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="5"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="5"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="5"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="5"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="5"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="5"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="5"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="5"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="5"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="5"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="5"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="A17" s="8">
         <v>16</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="11"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2612,244 +2606,244 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add On Hit and Die animation (#28)
* feat: add Sound Manager

* feat: add player On Hit animation

* feat: handle On Hit and Die event

* feat: Add die animation
</commit_message>
<xml_diff>
--- a/Excels/GameData.xlsx
+++ b/Excels/GameData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCMUS\Nam 4\Game\2D\The Transcendent Legend 2D\The Transcendent Legend 2D\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A597FBD4-FCA0-491F-9AA3-D38EEB780AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAF276A-7FAE-4C64-88EF-45D1B390322B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,8 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -46,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
   <si>
     <t>Id</t>
   </si>
@@ -175,6 +173,9 @@
   </si>
   <si>
     <t>SelfDamage</t>
+  </si>
+  <si>
+    <t>Health</t>
   </si>
 </sst>
 </file>
@@ -353,10 +354,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -370,6 +370,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1046,10 +1049,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1060,321 +1063,312 @@
     <col min="9" max="9" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="M1" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="12">
         <v>1</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="12">
         <v>1</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="12">
         <v>0</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="12">
         <v>1</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="12">
         <v>1</v>
       </c>
-      <c r="I2" s="13">
+      <c r="I2" s="12">
         <v>2</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="12">
         <v>80</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="12">
         <v>150</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
-        <v>2</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="15"/>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
-        <v>3</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="15"/>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
-        <v>4</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="15"/>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
-        <v>5</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="15"/>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
-        <v>6</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="15"/>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
-        <v>7</v>
-      </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="15"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
-        <v>8</v>
-      </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="15"/>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
-        <v>9</v>
-      </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="15"/>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
-        <v>10</v>
-      </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="15"/>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
-        <v>11</v>
-      </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="15"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="15"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
-        <v>13</v>
-      </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="15"/>
-    </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
-        <v>14</v>
-      </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="15"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13">
-        <v>15</v>
-      </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="15"/>
-    </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
-        <v>16</v>
-      </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="15"/>
+      <c r="M2" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1443,266 +1437,266 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2">
         <v>10</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1764,248 +1758,248 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2">
         <v>10</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2054,182 +2048,182 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2">
         <v>10</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2258,296 +2252,296 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>10</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>0</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>1</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>0</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="4">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>10</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>0</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>5</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>2</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="4">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="5"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="5"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="5"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="5"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="5"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="5"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="5"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="5"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="5"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="5"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="5"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="5"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="5"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="A17" s="8">
         <v>16</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="11"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2612,244 +2606,244 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add base ui manager (#34)
* feat: add damage logic

* fix: player get stuck wall

* chore: add dotween pro package

* feat: add start menu to chapter one scene and demo

* fix: stuck when jumping

* feat: handlle attack in Rat and Player

* fix: rat attack multiple times

* fix: player jump and add logic to play stats ui

* feat: back to main menu logic

* feat: Add base in game ui manager
fix: Coyate time and Die trigger
</commit_message>
<xml_diff>
--- a/Excels/GameData.xlsx
+++ b/Excels/GameData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCMUS\Nam 4\Game\2D\The Transcendent Legend 2D\The Transcendent Legend 2D\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAF276A-7FAE-4C64-88EF-45D1B390322B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBE1A53-2638-4134-B6BE-02662C619364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -354,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -370,7 +370,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -1052,7 +1051,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1094,13 +1093,13 @@
       <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="16" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1115,10 +1114,10 @@
         <v>13</v>
       </c>
       <c r="D2" s="12">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E2" s="12">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F2" s="12">
         <v>0</v>
@@ -1141,7 +1140,7 @@
       <c r="L2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="15">
+      <c r="M2" s="12">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add Skill UI
</commit_message>
<xml_diff>
--- a/Excels/GameData.xlsx
+++ b/Excels/GameData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCMUS\Nam 4\Game\2D\The Transcendent Legend 2D\The Transcendent Legend 2D\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBE1A53-2638-4134-B6BE-02662C619364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272FF25C-6F9C-4FFE-A0A9-C3CCAD08AA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="1" r:id="rId1"/>
@@ -1050,8 +1050,8 @@
   </sheetPr>
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1114,7 +1114,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="12">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E2" s="12">
         <v>20</v>
@@ -2236,8 +2236,8 @@
   </sheetPr>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add Toxic Skill UI (#45)
* Quick Fix rat not turn back

* feat: add Skill UI

* feat: add Skill UI
</commit_message>
<xml_diff>
--- a/Excels/GameData.xlsx
+++ b/Excels/GameData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCMUS\Nam 4\Game\2D\The Transcendent Legend 2D\The Transcendent Legend 2D\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBE1A53-2638-4134-B6BE-02662C619364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272FF25C-6F9C-4FFE-A0A9-C3CCAD08AA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="1" r:id="rId1"/>
@@ -1050,8 +1050,8 @@
   </sheetPr>
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1114,7 +1114,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="12">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E2" s="12">
         <v>20</v>
@@ -2236,8 +2236,8 @@
   </sheetPr>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>